<commit_message>
TP#20088: Update Freight missing members and spreadsheet
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Freight.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Freight.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwinchester\Documents\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="121">
   <si>
     <t>Revenue</t>
   </si>
@@ -363,12 +363,36 @@
   </si>
   <si>
     <t xml:space="preserve">Save Label </t>
+  </si>
+  <si>
+    <t>FreightClass2</t>
+  </si>
+  <si>
+    <t>Packaging2</t>
+  </si>
+  <si>
+    <t>Pieces2</t>
+  </si>
+  <si>
+    <t>Units2</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Length2</t>
+  </si>
+  <si>
+    <t>Width2</t>
+  </si>
+  <si>
+    <t>Height2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1976,6 +2000,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2011,6 +2052,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2195,7 +2253,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2624,31 +2682,31 @@
         <v>37</v>
       </c>
       <c r="BE2" s="6" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="BF2" s="6" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="BG2" s="6" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="BH2" s="6" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="BI2" s="6" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="BJ2" s="6" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="BK2" s="6" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="BL2" s="6" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="BM2" s="6" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="BN2" s="7" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
TP#20088: They had duplicate CustomerTransactionID values, so I made them equal to the ExpressLabel TC# which were unique.  These duplicates were causing saved labels to be overwritten by the last test run.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Freight.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Freight.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwinchester\Documents\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -392,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2000,23 +2000,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2052,23 +2035,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2253,7 +2219,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2749,8 +2715,8 @@
       <c r="E3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="43" t="s">
-        <v>55</v>
+      <c r="F3" s="41" t="s">
+        <v>54</v>
       </c>
       <c r="G3" s="43"/>
       <c r="H3" s="43" t="s">
@@ -2966,8 +2932,8 @@
       <c r="E4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>66</v>
+      <c r="F4" s="31" t="s">
+        <v>55</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="33" t="s">
@@ -3181,8 +3147,8 @@
       <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>55</v>
+      <c r="F5" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
@@ -3416,8 +3382,8 @@
       <c r="E6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>66</v>
+      <c r="F6" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">

</xml_diff>